<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 06:51
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211440</v>
+        <v>202509211451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:02
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211451</v>
+        <v>202509211502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:17
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211502</v>
+        <v>202509211517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:22
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211517</v>
+        <v>202509211522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:26
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211522</v>
+        <v>202509211526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:30
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211526</v>
+        <v>202509211530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:31
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211530</v>
+        <v>202509211531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:37
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211531</v>
+        <v>202509211537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:41
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211537</v>
+        <v>202509211541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:49
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211541</v>
+        <v>202509211549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:50
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211549</v>
+        <v>202509211550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 07:59
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211550</v>
+        <v>202509211559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 08:06
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211559</v>
+        <v>202509211606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 08:28
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>9.71</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>2.06</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>5.26</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>1.92</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>0.98</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>5.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>9.21</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>5.03</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>0.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.17</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>0.97</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>4.91</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>6.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>4.89</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>4.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>5.22</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>1.02</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>5.69</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>1.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.38</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>3.14</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>1.01</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +930,7 @@
         <v>6.85</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +953,7 @@
         <v>0.98</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +976,7 @@
         <v>5.05</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1045,7 @@
         <v>9.6</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
         <v>5.04</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211606</v>
+        <v>202509211628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 08:55
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,16 +426,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B2" t="str">
-        <v>000333</v>
+        <v>000089</v>
       </c>
       <c r="C2" t="str">
-        <v>美的集团</v>
+        <v>深圳机场</v>
       </c>
       <c r="D2">
-        <v>9.71</v>
+        <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="3">
@@ -443,16 +443,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B3" t="str">
-        <v>518880</v>
+        <v>000333</v>
       </c>
       <c r="C3" t="str">
-        <v>黄金ETF</v>
+        <v>美的集团</v>
       </c>
       <c r="D3">
-        <v>2.06</v>
+        <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="4">
@@ -460,16 +460,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B4" t="str">
-        <v>510300</v>
+        <v>000831</v>
       </c>
       <c r="C4" t="str">
-        <v>沪深300ETF</v>
+        <v>中国稀土</v>
       </c>
       <c r="D4">
-        <v>5.26</v>
+        <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="5">
@@ -477,16 +477,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B5" t="str">
-        <v>600085</v>
+        <v>510300</v>
       </c>
       <c r="C5" t="str">
-        <v>同仁堂</v>
+        <v>沪深300ETF</v>
       </c>
       <c r="D5">
-        <v>1.92</v>
+        <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="6">
@@ -494,16 +494,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B6" t="str">
-        <v>601899</v>
+        <v>513400</v>
       </c>
       <c r="C6" t="str">
-        <v>紫金矿业</v>
+        <v>道琼斯ETF</v>
       </c>
       <c r="D6">
-        <v>0.98</v>
+        <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="7">
@@ -511,16 +511,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B7" t="str">
-        <v>513400</v>
+        <v>518880</v>
       </c>
       <c r="C7" t="str">
-        <v>道琼斯ETF</v>
+        <v>黄金ETF</v>
       </c>
       <c r="D7">
-        <v>5.11</v>
+        <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="8">
@@ -528,16 +528,16 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B8" t="str">
-        <v>000831</v>
+        <v>600085</v>
       </c>
       <c r="C8" t="str">
-        <v>中国稀土</v>
+        <v>同仁堂</v>
       </c>
       <c r="D8">
-        <v>9.21</v>
+        <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="9">
@@ -545,28 +545,45 @@
         <v>大智 (稳健智远)</v>
       </c>
       <c r="B9" t="str">
-        <v>000089</v>
+        <v>601899</v>
       </c>
       <c r="C9" t="str">
-        <v>深圳机场</v>
+        <v>紫金矿业</v>
       </c>
       <c r="D9">
-        <v>5.03</v>
+        <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B10" t="str">
+        <v>100000</v>
+      </c>
+      <c r="C10" t="str">
+        <v>现金</v>
+      </c>
+      <c r="D10">
+        <v>60.73</v>
+      </c>
+      <c r="E10" t="str">
+        <v>202509211655</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -593,16 +610,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B2" t="str">
-        <v>603119</v>
+        <v>000725</v>
       </c>
       <c r="C2" t="str">
-        <v>浙江荣泰</v>
+        <v>京东方A</v>
       </c>
       <c r="D2">
-        <v>0.03</v>
+        <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="3">
@@ -610,16 +627,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B3" t="str">
-        <v>513100</v>
+        <v>001380</v>
       </c>
       <c r="C3" t="str">
-        <v>纳指ETF</v>
+        <v>华纬科技</v>
       </c>
       <c r="D3">
-        <v>5.17</v>
+        <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="4">
@@ -627,16 +644,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B4" t="str">
-        <v>513290</v>
+        <v>002074</v>
       </c>
       <c r="C4" t="str">
-        <v>纳指生物科技ETF</v>
+        <v>国轩高科</v>
       </c>
       <c r="D4">
-        <v>0.97</v>
+        <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="5">
@@ -644,16 +661,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B5" t="str">
-        <v>000725</v>
+        <v>159781</v>
       </c>
       <c r="C5" t="str">
-        <v>京东方A</v>
+        <v>科创创业ETF</v>
       </c>
       <c r="D5">
-        <v>4.91</v>
+        <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="6">
@@ -661,16 +678,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B6" t="str">
-        <v>159781</v>
+        <v>513100</v>
       </c>
       <c r="C6" t="str">
-        <v>科创创业ETF</v>
+        <v>纳指ETF</v>
       </c>
       <c r="D6">
-        <v>6.11</v>
+        <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="7">
@@ -678,16 +695,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B7" t="str">
-        <v>601878</v>
+        <v>513290</v>
       </c>
       <c r="C7" t="str">
-        <v>浙商证券</v>
+        <v>纳指生物科技ETF</v>
       </c>
       <c r="D7">
-        <v>4.89</v>
+        <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="8">
@@ -695,16 +712,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B8" t="str">
-        <v>002074</v>
+        <v>600580</v>
       </c>
       <c r="C8" t="str">
-        <v>国轩高科</v>
+        <v>卧龙电驱</v>
       </c>
       <c r="D8">
-        <v>4.75</v>
+        <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="9">
@@ -712,16 +729,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B9" t="str">
-        <v>001380</v>
+        <v>601878</v>
       </c>
       <c r="C9" t="str">
-        <v>华纬科技</v>
+        <v>浙商证券</v>
       </c>
       <c r="D9">
-        <v>5.22</v>
+        <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="10">
@@ -729,16 +746,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B10" t="str">
-        <v>HK01810</v>
+        <v>603119</v>
       </c>
       <c r="C10" t="str">
-        <v>小米集团-W</v>
+        <v>浙江荣泰</v>
       </c>
       <c r="D10">
-        <v>1.02</v>
+        <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="11">
@@ -746,28 +763,45 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B11" t="str">
-        <v>600580</v>
+        <v>HK01810</v>
       </c>
       <c r="C11" t="str">
-        <v>卧龙电驱</v>
+        <v>小米集团-W</v>
       </c>
       <c r="D11">
-        <v>5.69</v>
+        <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B12" t="str">
+        <v>100000</v>
+      </c>
+      <c r="C12" t="str">
+        <v>现金</v>
+      </c>
+      <c r="D12">
+        <v>61.24</v>
+      </c>
+      <c r="E12" t="str">
+        <v>202509211655</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -800,22 +834,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B2" t="str">
-        <v>000333</v>
+        <v>000089</v>
       </c>
       <c r="C2" t="str">
-        <v>美的集团</v>
+        <v>深圳机场</v>
       </c>
       <c r="D2" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E2">
-        <v>9.71</v>
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
       <c r="F2">
-        <v>1.01</v>
+        <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="3">
@@ -823,22 +857,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B3" t="str">
-        <v>518880</v>
+        <v>000333</v>
       </c>
       <c r="C3" t="str">
-        <v>黄金ETF</v>
+        <v>美的集团</v>
       </c>
       <c r="D3" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E3">
-        <v>2.04</v>
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="4">
@@ -846,22 +880,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B4" t="str">
-        <v>510300</v>
+        <v>000725</v>
       </c>
       <c r="C4" t="str">
-        <v>沪深300ETF</v>
+        <v>京东方A</v>
       </c>
       <c r="D4" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E4">
-        <v>5.28</v>
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
       </c>
       <c r="F4">
-        <v>5.38</v>
+        <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="5">
@@ -869,22 +903,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B5" t="str">
-        <v>513100</v>
+        <v>000831</v>
       </c>
       <c r="C5" t="str">
-        <v>纳指ETF</v>
+        <v>中国稀土</v>
       </c>
       <c r="D5" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E5">
-        <v>5.05</v>
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
       </c>
       <c r="F5">
-        <v>3.14</v>
+        <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="6">
@@ -892,22 +926,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B6" t="str">
-        <v>510050</v>
+        <v>159781</v>
       </c>
       <c r="C6" t="str">
-        <v>上证50ETF</v>
+        <v>科创创业ETF</v>
       </c>
       <c r="D6" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E6">
-        <v>5.14</v>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
       </c>
       <c r="F6">
-        <v>1.01</v>
+        <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="7">
@@ -915,22 +949,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B7" t="str">
-        <v>159781</v>
+        <v>510050</v>
       </c>
       <c r="C7" t="str">
-        <v>科创创业ETF</v>
+        <v>上证50ETF</v>
       </c>
       <c r="D7" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E7">
-        <v>6.13</v>
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
       </c>
       <c r="F7">
-        <v>6.85</v>
+        <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="8">
@@ -938,22 +972,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B8" t="str">
-        <v>600085</v>
+        <v>510300</v>
       </c>
       <c r="C8" t="str">
-        <v>同仁堂</v>
+        <v>沪深300ETF</v>
       </c>
       <c r="D8" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E8">
-        <v>1.91</v>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
       </c>
       <c r="F8">
-        <v>0.98</v>
+        <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="9">
@@ -961,22 +995,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B9" t="str">
-        <v>513400</v>
+        <v>513100</v>
       </c>
       <c r="C9" t="str">
-        <v>道琼斯ETF</v>
+        <v>纳指ETF</v>
       </c>
       <c r="D9" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E9">
-        <v>5.05</v>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <v/>
       </c>
       <c r="F9">
-        <v>5.05</v>
+        <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="10">
@@ -990,16 +1024,16 @@
         <v>纳指生物科技ETF</v>
       </c>
       <c r="D10" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E10">
-        <v>0.98</v>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v/>
       </c>
       <c r="F10">
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="11">
@@ -1007,22 +1041,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B11" t="str">
-        <v>000725</v>
+        <v>513400</v>
       </c>
       <c r="C11" t="str">
-        <v>京东方A</v>
+        <v>道琼斯ETF</v>
       </c>
       <c r="D11" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E11">
-        <v>4.96</v>
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <v/>
       </c>
       <c r="F11">
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="12">
@@ -1030,22 +1064,22 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B12" t="str">
-        <v>000831</v>
+        <v>518880</v>
       </c>
       <c r="C12" t="str">
-        <v>中国稀土</v>
+        <v>黄金ETF</v>
       </c>
       <c r="D12" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E12">
-        <v>9.86</v>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v/>
       </c>
       <c r="F12">
-        <v>9.6</v>
+        <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
       </c>
     </row>
     <row r="13">
@@ -1053,27 +1087,50 @@
         <v>范式进化投资组合</v>
       </c>
       <c r="B13" t="str">
-        <v>000089</v>
+        <v>600085</v>
       </c>
       <c r="C13" t="str">
-        <v>深圳机场</v>
+        <v>同仁堂</v>
       </c>
       <c r="D13" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <v/>
       </c>
       <c r="F13">
-        <v>5.04</v>
+        <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211628</v>
+        <v>202509211655</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B14" t="str">
+        <v>100000</v>
+      </c>
+      <c r="C14" t="str">
+        <v>现金</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14">
+        <v>54.9</v>
+      </c>
+      <c r="G14" t="str">
+        <v>202509211655</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 10:36
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="9">
@@ -554,36 +554,19 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211655</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B10" t="str">
-        <v>100000</v>
-      </c>
-      <c r="C10" t="str">
-        <v>现金</v>
-      </c>
-      <c r="D10">
-        <v>60.73</v>
-      </c>
-      <c r="E10" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -619,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="3">
@@ -636,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="4">
@@ -653,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="5">
@@ -670,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="6">
@@ -687,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="7">
@@ -704,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="8">
@@ -721,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="10">
@@ -755,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="11">
@@ -772,36 +755,19 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211655</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>大成 (锐进先锋)</v>
-      </c>
-      <c r="B12" t="str">
-        <v>100000</v>
-      </c>
-      <c r="C12" t="str">
-        <v>现金</v>
-      </c>
-      <c r="D12">
-        <v>61.24</v>
-      </c>
-      <c r="E12" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -840,16 +806,16 @@
         <v>深圳机场</v>
       </c>
       <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E2">
+        <v>5.03</v>
       </c>
       <c r="F2">
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="3">
@@ -863,16 +829,16 @@
         <v>美的集团</v>
       </c>
       <c r="D3" t="str">
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E3">
+        <v>9.71</v>
       </c>
       <c r="F3">
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="4">
@@ -886,16 +852,16 @@
         <v>京东方A</v>
       </c>
       <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
+        <v>大成</v>
+      </c>
+      <c r="E4">
+        <v>4.91</v>
       </c>
       <c r="F4">
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="5">
@@ -909,16 +875,16 @@
         <v>中国稀土</v>
       </c>
       <c r="D5" t="str">
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E5">
+        <v>9.21</v>
       </c>
       <c r="F5">
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="6">
@@ -932,16 +898,16 @@
         <v>科创创业ETF</v>
       </c>
       <c r="D6" t="str">
-        <v/>
-      </c>
-      <c r="E6" t="str">
-        <v/>
+        <v>大成</v>
+      </c>
+      <c r="E6">
+        <v>6.11</v>
       </c>
       <c r="F6">
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="7">
@@ -957,14 +923,14 @@
       <c r="D7" t="str">
         <v/>
       </c>
-      <c r="E7" t="str">
-        <v/>
+      <c r="E7">
+        <v>NaN</v>
       </c>
       <c r="F7">
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="8">
@@ -978,16 +944,16 @@
         <v>沪深300ETF</v>
       </c>
       <c r="D8" t="str">
-        <v/>
-      </c>
-      <c r="E8" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E8">
+        <v>5.26</v>
       </c>
       <c r="F8">
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="9">
@@ -1001,16 +967,16 @@
         <v>纳指ETF</v>
       </c>
       <c r="D9" t="str">
-        <v/>
-      </c>
-      <c r="E9" t="str">
-        <v/>
+        <v>大成</v>
+      </c>
+      <c r="E9">
+        <v>5.17</v>
       </c>
       <c r="F9">
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="10">
@@ -1024,16 +990,16 @@
         <v>纳指生物科技ETF</v>
       </c>
       <c r="D10" t="str">
-        <v/>
-      </c>
-      <c r="E10" t="str">
-        <v/>
+        <v>大成</v>
+      </c>
+      <c r="E10">
+        <v>0.97</v>
       </c>
       <c r="F10">
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="11">
@@ -1047,16 +1013,16 @@
         <v>道琼斯ETF</v>
       </c>
       <c r="D11" t="str">
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E11">
+        <v>5.11</v>
       </c>
       <c r="F11">
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="12">
@@ -1070,16 +1036,16 @@
         <v>黄金ETF</v>
       </c>
       <c r="D12" t="str">
-        <v/>
-      </c>
-      <c r="E12" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E12">
+        <v>2.06</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
     <row r="13">
@@ -1093,44 +1059,21 @@
         <v>同仁堂</v>
       </c>
       <c r="D13" t="str">
-        <v/>
-      </c>
-      <c r="E13" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E13">
+        <v>1.92</v>
       </c>
       <c r="F13">
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211655</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B14" t="str">
-        <v>100000</v>
-      </c>
-      <c r="C14" t="str">
-        <v>现金</v>
-      </c>
-      <c r="D14" t="str">
-        <v/>
-      </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
-      <c r="F14">
-        <v>54.9</v>
-      </c>
-      <c r="G14" t="str">
-        <v>202509211655</v>
+        <v>202509211836</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 11:02
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="7">
@@ -923,14 +923,11 @@
       <c r="D7" t="str">
         <v/>
       </c>
-      <c r="E7">
-        <v>NaN</v>
-      </c>
       <c r="F7">
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +950,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +973,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +996,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1019,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1065,7 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211836</v>
+        <v>202509211902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 12:22
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="7">
@@ -927,7 +927,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="9">
@@ -973,7 +973,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="10">
@@ -996,7 +996,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="11">
@@ -1019,7 +1019,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="12">
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
     <row r="13">
@@ -1065,7 +1065,7 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509211902</v>
+        <v>202509212022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 14:46
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="7">
@@ -927,7 +927,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="9">
@@ -973,7 +973,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="10">
@@ -996,7 +996,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="11">
@@ -1019,7 +1019,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="12">
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
     <row r="13">
@@ -1065,7 +1065,7 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509212022</v>
+        <v>2025-09-21 22:46:47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 15:05
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="7">
@@ -927,7 +927,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="9">
@@ -973,7 +973,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="10">
@@ -996,7 +996,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="11">
@@ -1019,7 +1019,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="12">
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
     <row r="13">
@@ -1065,7 +1065,7 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>2025-09-21 22:46:47</v>
+        <v>202509212305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 16:07
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.91</v>
       </c>
       <c r="E2" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.22</v>
       </c>
       <c r="E3" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.75</v>
       </c>
       <c r="E4" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.11</v>
       </c>
       <c r="E5" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.17</v>
       </c>
       <c r="E6" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.69</v>
       </c>
       <c r="E8" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>4.89</v>
       </c>
       <c r="E9" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>1.02</v>
       </c>
       <c r="E11" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +907,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="7">
@@ -921,13 +921,16 @@
         <v>上证50ETF</v>
       </c>
       <c r="D7" t="str">
-        <v/>
+        <v>大智</v>
+      </c>
+      <c r="E7">
+        <v>5.14</v>
       </c>
       <c r="F7">
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +953,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="9">
@@ -973,7 +976,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="10">
@@ -996,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="11">
@@ -1019,7 +1022,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="12">
@@ -1042,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
     <row r="13">
@@ -1065,7 +1068,7 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509212305</v>
+        <v>202509220007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-21 16:10
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -399,173 +399,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>组合名称</v>
-      </c>
-      <c r="B1" t="str">
-        <v>股票代码</v>
-      </c>
-      <c r="C1" t="str">
-        <v>股票名称</v>
-      </c>
-      <c r="D1" t="str">
-        <v>配置比例 (%)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>修改时间</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B2" t="str">
-        <v>000089</v>
-      </c>
-      <c r="C2" t="str">
-        <v>深圳机场</v>
-      </c>
-      <c r="D2">
-        <v>5.03</v>
-      </c>
-      <c r="E2" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B3" t="str">
-        <v>000333</v>
-      </c>
-      <c r="C3" t="str">
-        <v>美的集团</v>
-      </c>
-      <c r="D3">
-        <v>9.71</v>
-      </c>
-      <c r="E3" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B4" t="str">
-        <v>000831</v>
-      </c>
-      <c r="C4" t="str">
-        <v>中国稀土</v>
-      </c>
-      <c r="D4">
-        <v>9.21</v>
-      </c>
-      <c r="E4" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B5" t="str">
-        <v>510300</v>
-      </c>
-      <c r="C5" t="str">
-        <v>沪深300ETF</v>
-      </c>
-      <c r="D5">
-        <v>5.26</v>
-      </c>
-      <c r="E5" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B6" t="str">
-        <v>513400</v>
-      </c>
-      <c r="C6" t="str">
-        <v>道琼斯ETF</v>
-      </c>
-      <c r="D6">
-        <v>5.11</v>
-      </c>
-      <c r="E6" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B7" t="str">
-        <v>518880</v>
-      </c>
-      <c r="C7" t="str">
-        <v>黄金ETF</v>
-      </c>
-      <c r="D7">
-        <v>2.06</v>
-      </c>
-      <c r="E7" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B8" t="str">
-        <v>600085</v>
-      </c>
-      <c r="C8" t="str">
-        <v>同仁堂</v>
-      </c>
-      <c r="D8">
-        <v>1.92</v>
-      </c>
-      <c r="E8" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B9" t="str">
-        <v>601899</v>
-      </c>
-      <c r="C9" t="str">
-        <v>紫金矿业</v>
-      </c>
-      <c r="D9">
-        <v>0.98</v>
-      </c>
-      <c r="E9" t="str">
-        <v>202509220007</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -590,172 +423,172 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B2" t="str">
-        <v>000725</v>
+        <v>000089</v>
       </c>
       <c r="C2" t="str">
-        <v>京东方A</v>
+        <v>深圳机场</v>
       </c>
       <c r="D2">
-        <v>4.91</v>
+        <v>5.03</v>
       </c>
       <c r="E2" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B3" t="str">
-        <v>001380</v>
+        <v>000333</v>
       </c>
       <c r="C3" t="str">
-        <v>华纬科技</v>
+        <v>美的集团</v>
       </c>
       <c r="D3">
-        <v>5.22</v>
+        <v>9.71</v>
       </c>
       <c r="E3" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B4" t="str">
-        <v>002074</v>
+        <v>000831</v>
       </c>
       <c r="C4" t="str">
-        <v>国轩高科</v>
+        <v>中国稀土</v>
       </c>
       <c r="D4">
-        <v>4.75</v>
+        <v>9.21</v>
       </c>
       <c r="E4" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B5" t="str">
-        <v>159781</v>
+        <v>510300</v>
       </c>
       <c r="C5" t="str">
-        <v>科创创业ETF</v>
+        <v>沪深300ETF</v>
       </c>
       <c r="D5">
-        <v>6.11</v>
+        <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B6" t="str">
-        <v>513100</v>
+        <v>513400</v>
       </c>
       <c r="C6" t="str">
-        <v>纳指ETF</v>
+        <v>道琼斯ETF</v>
       </c>
       <c r="D6">
-        <v>5.17</v>
+        <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B7" t="str">
-        <v>513290</v>
+        <v>518880</v>
       </c>
       <c r="C7" t="str">
-        <v>纳指生物科技ETF</v>
+        <v>黄金ETF</v>
       </c>
       <c r="D7">
-        <v>0.97</v>
+        <v>2.06</v>
       </c>
       <c r="E7" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B8" t="str">
-        <v>600580</v>
+        <v>600085</v>
       </c>
       <c r="C8" t="str">
-        <v>卧龙电驱</v>
+        <v>同仁堂</v>
       </c>
       <c r="D8">
-        <v>5.69</v>
+        <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B9" t="str">
-        <v>601878</v>
+        <v>601899</v>
       </c>
       <c r="C9" t="str">
-        <v>浙商证券</v>
+        <v>紫金矿业</v>
       </c>
       <c r="D9">
-        <v>4.89</v>
+        <v>0.98</v>
       </c>
       <c r="E9" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B10" t="str">
-        <v>603119</v>
+        <v>603391</v>
       </c>
       <c r="C10" t="str">
-        <v>浙江荣泰</v>
+        <v>力聚热能</v>
       </c>
       <c r="D10">
-        <v>0.03</v>
+        <v>26.47</v>
       </c>
       <c r="E10" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>大成 (锐进先锋)</v>
+        <v>大智 (稳健智远)</v>
       </c>
       <c r="B11" t="str">
-        <v>HK01810</v>
+        <v>002555</v>
       </c>
       <c r="C11" t="str">
-        <v>小米集团-W</v>
+        <v>三七互娱</v>
       </c>
       <c r="D11">
-        <v>1.02</v>
+        <v>14.71</v>
       </c>
       <c r="E11" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
   </sheetData>
@@ -765,9 +598,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -783,6 +616,258 @@
         <v>股票名称</v>
       </c>
       <c r="D1" t="str">
+        <v>配置比例 (%)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>修改时间</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B2" t="str">
+        <v>000725</v>
+      </c>
+      <c r="C2" t="str">
+        <v>京东方A</v>
+      </c>
+      <c r="D2">
+        <v>4.91</v>
+      </c>
+      <c r="E2" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B3" t="str">
+        <v>001380</v>
+      </c>
+      <c r="C3" t="str">
+        <v>华纬科技</v>
+      </c>
+      <c r="D3">
+        <v>5.22</v>
+      </c>
+      <c r="E3" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B4" t="str">
+        <v>002074</v>
+      </c>
+      <c r="C4" t="str">
+        <v>国轩高科</v>
+      </c>
+      <c r="D4">
+        <v>4.75</v>
+      </c>
+      <c r="E4" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B5" t="str">
+        <v>159781</v>
+      </c>
+      <c r="C5" t="str">
+        <v>科创创业ETF</v>
+      </c>
+      <c r="D5">
+        <v>6.11</v>
+      </c>
+      <c r="E5" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B6" t="str">
+        <v>513100</v>
+      </c>
+      <c r="C6" t="str">
+        <v>纳指ETF</v>
+      </c>
+      <c r="D6">
+        <v>5.17</v>
+      </c>
+      <c r="E6" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B7" t="str">
+        <v>513290</v>
+      </c>
+      <c r="C7" t="str">
+        <v>纳指生物科技ETF</v>
+      </c>
+      <c r="D7">
+        <v>0.97</v>
+      </c>
+      <c r="E7" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B8" t="str">
+        <v>600580</v>
+      </c>
+      <c r="C8" t="str">
+        <v>卧龙电驱</v>
+      </c>
+      <c r="D8">
+        <v>5.69</v>
+      </c>
+      <c r="E8" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B9" t="str">
+        <v>601878</v>
+      </c>
+      <c r="C9" t="str">
+        <v>浙商证券</v>
+      </c>
+      <c r="D9">
+        <v>4.89</v>
+      </c>
+      <c r="E9" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B10" t="str">
+        <v>603119</v>
+      </c>
+      <c r="C10" t="str">
+        <v>浙江荣泰</v>
+      </c>
+      <c r="D10">
+        <v>0.03</v>
+      </c>
+      <c r="E10" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B11" t="str">
+        <v>HK01810</v>
+      </c>
+      <c r="C11" t="str">
+        <v>小米集团-W</v>
+      </c>
+      <c r="D11">
+        <v>1.02</v>
+      </c>
+      <c r="E11" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B12" t="str">
+        <v>601598</v>
+      </c>
+      <c r="C12" t="str">
+        <v>中国外运</v>
+      </c>
+      <c r="D12">
+        <v>27.01</v>
+      </c>
+      <c r="E12" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B13" t="str">
+        <v>603301</v>
+      </c>
+      <c r="C13" t="str">
+        <v>振德医疗</v>
+      </c>
+      <c r="D13">
+        <v>9.69</v>
+      </c>
+      <c r="E13" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B14" t="str">
+        <v>000014</v>
+      </c>
+      <c r="C14" t="str">
+        <v>沙河股份</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>组合名称</v>
+      </c>
+      <c r="B1" t="str">
+        <v>股票代码</v>
+      </c>
+      <c r="C1" t="str">
+        <v>股票名称</v>
+      </c>
+      <c r="D1" t="str">
         <v>来源</v>
       </c>
       <c r="E1" t="str">
@@ -815,7 +900,7 @@
         <v>5.04</v>
       </c>
       <c r="G2" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +923,7 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +946,7 @@
         <v>5.05</v>
       </c>
       <c r="G4" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +969,7 @@
         <v>9.6</v>
       </c>
       <c r="G5" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="6">
@@ -907,7 +992,7 @@
         <v>6.85</v>
       </c>
       <c r="G6" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="7">
@@ -930,7 +1015,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +1038,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +1061,7 @@
         <v>3.14</v>
       </c>
       <c r="G9" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="10">
@@ -999,7 +1084,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="11">
@@ -1022,7 +1107,7 @@
         <v>5.05</v>
       </c>
       <c r="G11" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="12">
@@ -1045,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
       </c>
     </row>
     <row r="13">
@@ -1068,12 +1153,127 @@
         <v>0.98</v>
       </c>
       <c r="G13" t="str">
-        <v>202509220007</v>
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B14" t="str">
+        <v>603391</v>
+      </c>
+      <c r="C14" t="str">
+        <v>力聚热能</v>
+      </c>
+      <c r="D14" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E14">
+        <v>26.47</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B15" t="str">
+        <v>002555</v>
+      </c>
+      <c r="C15" t="str">
+        <v>三七互娱</v>
+      </c>
+      <c r="D15" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E15">
+        <v>14.71</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B16" t="str">
+        <v>601598</v>
+      </c>
+      <c r="C16" t="str">
+        <v>中国外运</v>
+      </c>
+      <c r="D16" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E16">
+        <v>27.01</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B17" t="str">
+        <v>603301</v>
+      </c>
+      <c r="C17" t="str">
+        <v>振德医疗</v>
+      </c>
+      <c r="D17" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E17">
+        <v>9.69</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="str">
+        <v>202509220010</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B18" t="str">
+        <v>000014</v>
+      </c>
+      <c r="C18" t="str">
+        <v>沙河股份</v>
+      </c>
+      <c r="D18" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
+      <c r="G18" t="str">
+        <v>202509220010</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-23 01:53
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -432,10 +432,10 @@
         <v>深圳机场</v>
       </c>
       <c r="D2">
-        <v>5.03</v>
+        <v>5.01</v>
       </c>
       <c r="E2" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="3">
@@ -449,10 +449,10 @@
         <v>美的集团</v>
       </c>
       <c r="D3">
-        <v>9.71</v>
+        <v>9.57</v>
       </c>
       <c r="E3" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="4">
@@ -466,10 +466,10 @@
         <v>中国稀土</v>
       </c>
       <c r="D4">
-        <v>9.21</v>
+        <v>9.22</v>
       </c>
       <c r="E4" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>沪深300ETF</v>
       </c>
       <c r="D5">
-        <v>5.26</v>
+        <v>5.28</v>
       </c>
       <c r="E5" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.11</v>
       </c>
       <c r="E6" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         <v>黄金ETF</v>
       </c>
       <c r="D7">
-        <v>2.06</v>
+        <v>2.1</v>
       </c>
       <c r="E7" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="8">
@@ -534,10 +534,10 @@
         <v>同仁堂</v>
       </c>
       <c r="D8">
-        <v>1.92</v>
+        <v>1.91</v>
       </c>
       <c r="E8" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="9">
@@ -551,56 +551,22 @@
         <v>紫金矿业</v>
       </c>
       <c r="D9">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="E9" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B10" t="str">
-        <v>603391</v>
-      </c>
-      <c r="C10" t="str">
-        <v>力聚热能</v>
-      </c>
-      <c r="D10">
-        <v>26.47</v>
-      </c>
-      <c r="E10" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>大智 (稳健智远)</v>
-      </c>
-      <c r="B11" t="str">
-        <v>002555</v>
-      </c>
-      <c r="C11" t="str">
-        <v>三七互娱</v>
-      </c>
-      <c r="D11">
-        <v>14.71</v>
-      </c>
-      <c r="E11" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -633,10 +599,10 @@
         <v>京东方A</v>
       </c>
       <c r="D2">
-        <v>4.91</v>
+        <v>4.9</v>
       </c>
       <c r="E2" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="3">
@@ -650,10 +616,10 @@
         <v>华纬科技</v>
       </c>
       <c r="D3">
-        <v>5.22</v>
+        <v>5.3</v>
       </c>
       <c r="E3" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="4">
@@ -667,10 +633,10 @@
         <v>国轩高科</v>
       </c>
       <c r="D4">
-        <v>4.75</v>
+        <v>4.8</v>
       </c>
       <c r="E4" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="5">
@@ -684,10 +650,10 @@
         <v>科创创业ETF</v>
       </c>
       <c r="D5">
-        <v>6.11</v>
+        <v>6.15</v>
       </c>
       <c r="E5" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="6">
@@ -701,10 +667,10 @@
         <v>纳指ETF</v>
       </c>
       <c r="D6">
-        <v>5.17</v>
+        <v>5.21</v>
       </c>
       <c r="E6" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="7">
@@ -718,10 +684,10 @@
         <v>纳指生物科技ETF</v>
       </c>
       <c r="D7">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="E7" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="8">
@@ -735,10 +701,10 @@
         <v>卧龙电驱</v>
       </c>
       <c r="D8">
-        <v>5.69</v>
+        <v>5.75</v>
       </c>
       <c r="E8" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="9">
@@ -752,10 +718,10 @@
         <v>浙商证券</v>
       </c>
       <c r="D9">
-        <v>4.89</v>
+        <v>4.88</v>
       </c>
       <c r="E9" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="10">
@@ -772,7 +738,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="11">
@@ -786,10 +752,10 @@
         <v>小米集团-W</v>
       </c>
       <c r="D11">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="E11" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="12">
@@ -797,16 +763,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B12" t="str">
-        <v>601598</v>
+        <v>605580</v>
       </c>
       <c r="C12" t="str">
-        <v>中国外运</v>
+        <v>恒盛能源</v>
       </c>
       <c r="D12">
-        <v>27.01</v>
+        <v>17.46</v>
       </c>
       <c r="E12" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="13">
@@ -814,45 +780,28 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B13" t="str">
-        <v>603301</v>
+        <v>601598</v>
       </c>
       <c r="C13" t="str">
-        <v>振德医疗</v>
+        <v>中国外运</v>
       </c>
       <c r="D13">
-        <v>9.69</v>
+        <v>32.09</v>
       </c>
       <c r="E13" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>大成 (锐进先锋)</v>
-      </c>
-      <c r="B14" t="str">
-        <v>000014</v>
-      </c>
-      <c r="C14" t="str">
-        <v>沙河股份</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E13"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -894,13 +843,13 @@
         <v>大智</v>
       </c>
       <c r="E2">
-        <v>5.03</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>5.04</v>
+        <v>5.01</v>
       </c>
       <c r="G2" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="3">
@@ -920,10 +869,10 @@
         <v>9.71</v>
       </c>
       <c r="F3">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="G3" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="4">
@@ -940,13 +889,13 @@
         <v>大成</v>
       </c>
       <c r="E4">
-        <v>4.91</v>
+        <v>4.96</v>
       </c>
       <c r="F4">
-        <v>5.05</v>
+        <v>5.06</v>
       </c>
       <c r="G4" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="5">
@@ -963,13 +912,13 @@
         <v>大智</v>
       </c>
       <c r="E5">
-        <v>9.21</v>
+        <v>9.86</v>
       </c>
       <c r="F5">
-        <v>9.6</v>
+        <v>9.59</v>
       </c>
       <c r="G5" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="6">
@@ -986,13 +935,13 @@
         <v>大成</v>
       </c>
       <c r="E6">
-        <v>6.11</v>
+        <v>6.13</v>
       </c>
       <c r="F6">
-        <v>6.85</v>
+        <v>6.92</v>
       </c>
       <c r="G6" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="7">
@@ -1015,7 +964,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="8">
@@ -1032,13 +981,13 @@
         <v>大智</v>
       </c>
       <c r="E8">
-        <v>5.26</v>
+        <v>5.28</v>
       </c>
       <c r="F8">
-        <v>5.38</v>
+        <v>5.4</v>
       </c>
       <c r="G8" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="9">
@@ -1055,13 +1004,13 @@
         <v>大成</v>
       </c>
       <c r="E9">
-        <v>5.17</v>
+        <v>5.05</v>
       </c>
       <c r="F9">
-        <v>3.14</v>
+        <v>3.18</v>
       </c>
       <c r="G9" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="10">
@@ -1078,13 +1027,13 @@
         <v>大成</v>
       </c>
       <c r="E10">
+        <v>0.98</v>
+      </c>
+      <c r="F10">
         <v>0.97</v>
       </c>
-      <c r="F10">
-        <v>0.98</v>
-      </c>
       <c r="G10" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="11">
@@ -1101,13 +1050,13 @@
         <v>大智</v>
       </c>
       <c r="E11">
-        <v>5.11</v>
+        <v>5.05</v>
       </c>
       <c r="F11">
-        <v>5.05</v>
+        <v>5.04</v>
       </c>
       <c r="G11" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="12">
@@ -1124,13 +1073,13 @@
         <v>大智</v>
       </c>
       <c r="E12">
-        <v>2.06</v>
+        <v>2.04</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="G12" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
     <row r="13">
@@ -1147,133 +1096,18 @@
         <v>大智</v>
       </c>
       <c r="E13">
-        <v>1.92</v>
+        <v>1.91</v>
       </c>
       <c r="F13">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="G13" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B14" t="str">
-        <v>603391</v>
-      </c>
-      <c r="C14" t="str">
-        <v>力聚热能</v>
-      </c>
-      <c r="D14" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E14">
-        <v>26.47</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B15" t="str">
-        <v>002555</v>
-      </c>
-      <c r="C15" t="str">
-        <v>三七互娱</v>
-      </c>
-      <c r="D15" t="str">
-        <v>大智</v>
-      </c>
-      <c r="E15">
-        <v>14.71</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
-      <c r="G15" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B16" t="str">
-        <v>601598</v>
-      </c>
-      <c r="C16" t="str">
-        <v>中国外运</v>
-      </c>
-      <c r="D16" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E16">
-        <v>27.01</v>
-      </c>
-      <c r="F16">
-        <v>13</v>
-      </c>
-      <c r="G16" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B17" t="str">
-        <v>603301</v>
-      </c>
-      <c r="C17" t="str">
-        <v>振德医疗</v>
-      </c>
-      <c r="D17" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E17">
-        <v>9.69</v>
-      </c>
-      <c r="F17">
-        <v>4</v>
-      </c>
-      <c r="G17" t="str">
-        <v>202509220010</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>范式进化投资组合</v>
-      </c>
-      <c r="B18" t="str">
-        <v>000014</v>
-      </c>
-      <c r="C18" t="str">
-        <v>沙河股份</v>
-      </c>
-      <c r="D18" t="str">
-        <v>大成</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1.5</v>
-      </c>
-      <c r="G18" t="str">
-        <v>202509220010</v>
+        <v>202509230952</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-24 02:08
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -432,10 +432,10 @@
         <v>深圳机场</v>
       </c>
       <c r="D2">
-        <v>5.01</v>
+        <v>5.06</v>
       </c>
       <c r="E2" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="3">
@@ -449,10 +449,10 @@
         <v>美的集团</v>
       </c>
       <c r="D3">
-        <v>9.57</v>
+        <v>9.61</v>
       </c>
       <c r="E3" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="4">
@@ -466,10 +466,10 @@
         <v>中国稀土</v>
       </c>
       <c r="D4">
-        <v>9.22</v>
+        <v>8.92</v>
       </c>
       <c r="E4" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>沪深300ETF</v>
       </c>
       <c r="D5">
-        <v>5.28</v>
+        <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="6">
@@ -500,10 +500,10 @@
         <v>道琼斯ETF</v>
       </c>
       <c r="D6">
-        <v>5.11</v>
+        <v>5.13</v>
       </c>
       <c r="E6" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         <v>黄金ETF</v>
       </c>
       <c r="D7">
-        <v>2.1</v>
+        <v>2.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="8">
@@ -534,10 +534,10 @@
         <v>同仁堂</v>
       </c>
       <c r="D8">
-        <v>1.91</v>
+        <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.99</v>
       </c>
       <c r="E9" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +566,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -602,7 +602,7 @@
         <v>4.9</v>
       </c>
       <c r="E2" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="3">
@@ -616,10 +616,10 @@
         <v>华纬科技</v>
       </c>
       <c r="D3">
-        <v>5.3</v>
+        <v>5.44</v>
       </c>
       <c r="E3" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="4">
@@ -633,10 +633,10 @@
         <v>国轩高科</v>
       </c>
       <c r="D4">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="E4" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="5">
@@ -650,10 +650,10 @@
         <v>科创创业ETF</v>
       </c>
       <c r="D5">
-        <v>6.15</v>
+        <v>6.14</v>
       </c>
       <c r="E5" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="6">
@@ -667,10 +667,10 @@
         <v>纳指ETF</v>
       </c>
       <c r="D6">
-        <v>5.21</v>
+        <v>5.23</v>
       </c>
       <c r="E6" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="7">
@@ -684,10 +684,10 @@
         <v>纳指生物科技ETF</v>
       </c>
       <c r="D7">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="8">
@@ -701,10 +701,10 @@
         <v>卧龙电驱</v>
       </c>
       <c r="D8">
-        <v>5.75</v>
+        <v>5.89</v>
       </c>
       <c r="E8" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="9">
@@ -712,16 +712,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B9" t="str">
-        <v>601878</v>
+        <v>601598</v>
       </c>
       <c r="C9" t="str">
-        <v>浙商证券</v>
+        <v>中国外运</v>
       </c>
       <c r="D9">
-        <v>4.88</v>
+        <v>32.01</v>
       </c>
       <c r="E9" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="10">
@@ -729,16 +729,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B10" t="str">
-        <v>603119</v>
+        <v>601878</v>
       </c>
       <c r="C10" t="str">
-        <v>浙江荣泰</v>
+        <v>浙商证券</v>
       </c>
       <c r="D10">
-        <v>0.03</v>
+        <v>4.85</v>
       </c>
       <c r="E10" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="11">
@@ -746,16 +746,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B11" t="str">
-        <v>HK01810</v>
+        <v>603119</v>
       </c>
       <c r="C11" t="str">
-        <v>小米集团-W</v>
+        <v>浙江荣泰</v>
       </c>
       <c r="D11">
-        <v>1.01</v>
+        <v>0.03</v>
       </c>
       <c r="E11" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="12">
@@ -763,38 +763,21 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B12" t="str">
-        <v>605580</v>
+        <v>HK01810</v>
       </c>
       <c r="C12" t="str">
-        <v>恒盛能源</v>
+        <v>小米集团-W</v>
       </c>
       <c r="D12">
-        <v>17.46</v>
+        <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>202509230952</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>大成 (锐进先锋)</v>
-      </c>
-      <c r="B13" t="str">
-        <v>601598</v>
-      </c>
-      <c r="C13" t="str">
-        <v>中国外运</v>
-      </c>
-      <c r="D13">
-        <v>32.09</v>
-      </c>
-      <c r="E13" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -846,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <v>5.01</v>
+        <v>5.06</v>
       </c>
       <c r="G2" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="3">
@@ -872,7 +855,7 @@
         <v>0.99</v>
       </c>
       <c r="G3" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="4">
@@ -892,10 +875,10 @@
         <v>4.96</v>
       </c>
       <c r="F4">
-        <v>5.06</v>
+        <v>5.08</v>
       </c>
       <c r="G4" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="5">
@@ -915,10 +898,10 @@
         <v>9.86</v>
       </c>
       <c r="F5">
-        <v>9.59</v>
+        <v>9.28</v>
       </c>
       <c r="G5" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="6">
@@ -938,10 +921,10 @@
         <v>6.13</v>
       </c>
       <c r="F6">
-        <v>6.92</v>
+        <v>6.94</v>
       </c>
       <c r="G6" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="7">
@@ -964,7 +947,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="8">
@@ -984,10 +967,10 @@
         <v>5.28</v>
       </c>
       <c r="F8">
-        <v>5.4</v>
+        <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="9">
@@ -1007,10 +990,10 @@
         <v>5.05</v>
       </c>
       <c r="F9">
-        <v>3.18</v>
+        <v>3.21</v>
       </c>
       <c r="G9" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="10">
@@ -1030,10 +1013,10 @@
         <v>0.98</v>
       </c>
       <c r="F10">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="11">
@@ -1053,10 +1036,10 @@
         <v>5.05</v>
       </c>
       <c r="F11">
-        <v>5.04</v>
+        <v>5.06</v>
       </c>
       <c r="G11" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="12">
@@ -1079,7 +1062,7 @@
         <v>1.02</v>
       </c>
       <c r="G12" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
     <row r="13">
@@ -1102,7 +1085,7 @@
         <v>0.97</v>
       </c>
       <c r="G13" t="str">
-        <v>202509230952</v>
+        <v>202509241007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-24 03:21
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.06</v>
       </c>
       <c r="E2" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.61</v>
       </c>
       <c r="E3" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>8.92</v>
       </c>
       <c r="E4" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>5.26</v>
       </c>
       <c r="E5" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.13</v>
       </c>
       <c r="E6" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.99</v>
       </c>
       <c r="E9" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>4.9</v>
       </c>
       <c r="E2" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.44</v>
       </c>
       <c r="E3" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>4.7</v>
       </c>
       <c r="E4" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.14</v>
       </c>
       <c r="E5" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         <v>5.23</v>
       </c>
       <c r="E6" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         <v>5.89</v>
       </c>
       <c r="E8" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="9">
@@ -718,10 +718,10 @@
         <v>中国外运</v>
       </c>
       <c r="D9">
-        <v>32.01</v>
+        <v>20</v>
       </c>
       <c r="E9" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="10">
@@ -738,7 +738,7 @@
         <v>4.85</v>
       </c>
       <c r="E10" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         <v>0.03</v>
       </c>
       <c r="E11" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="12">
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +832,7 @@
         <v>5.06</v>
       </c>
       <c r="G2" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="3">
@@ -855,7 +855,7 @@
         <v>0.99</v>
       </c>
       <c r="G3" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="4">
@@ -878,7 +878,7 @@
         <v>5.08</v>
       </c>
       <c r="G4" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="5">
@@ -901,7 +901,7 @@
         <v>9.28</v>
       </c>
       <c r="G5" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="6">
@@ -924,7 +924,7 @@
         <v>6.94</v>
       </c>
       <c r="G6" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="7">
@@ -947,7 +947,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="8">
@@ -970,7 +970,7 @@
         <v>5.38</v>
       </c>
       <c r="G8" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="9">
@@ -993,7 +993,7 @@
         <v>3.21</v>
       </c>
       <c r="G9" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="10">
@@ -1016,7 +1016,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="11">
@@ -1039,7 +1039,7 @@
         <v>5.06</v>
       </c>
       <c r="G11" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="12">
@@ -1062,7 +1062,7 @@
         <v>1.02</v>
       </c>
       <c r="G12" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
     <row r="13">
@@ -1085,7 +1085,7 @@
         <v>0.97</v>
       </c>
       <c r="G13" t="str">
-        <v>202509241007</v>
+        <v>202509241121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 通过 Web UI 更新投资组合数据于 2025-09-24 17:37
</commit_message>
<xml_diff>
--- a/data/AIPEPortfolio_new.xlsx
+++ b/data/AIPEPortfolio_new.xlsx
@@ -435,7 +435,7 @@
         <v>5.06</v>
       </c>
       <c r="E2" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +452,7 @@
         <v>9.61</v>
       </c>
       <c r="E3" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>8.92</v>
       </c>
       <c r="E4" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>沪深300ETF</v>
       </c>
       <c r="D5">
-        <v>5.26</v>
+        <v>5.27</v>
       </c>
       <c r="E5" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>5.13</v>
       </c>
       <c r="E6" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>2.11</v>
       </c>
       <c r="E7" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="8">
@@ -537,7 +537,7 @@
         <v>1.92</v>
       </c>
       <c r="E8" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="9">
@@ -554,7 +554,7 @@
         <v>0.99</v>
       </c>
       <c r="E9" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +566,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -599,10 +599,10 @@
         <v>京东方A</v>
       </c>
       <c r="D2">
-        <v>4.9</v>
+        <v>4.92</v>
       </c>
       <c r="E2" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="3">
@@ -619,7 +619,7 @@
         <v>5.44</v>
       </c>
       <c r="E3" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="4">
@@ -633,10 +633,10 @@
         <v>国轩高科</v>
       </c>
       <c r="D4">
-        <v>4.7</v>
+        <v>4.74</v>
       </c>
       <c r="E4" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         <v>6.14</v>
       </c>
       <c r="E5" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="6">
@@ -667,10 +667,10 @@
         <v>纳指ETF</v>
       </c>
       <c r="D6">
-        <v>5.23</v>
+        <v>5.2</v>
       </c>
       <c r="E6" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="7">
@@ -687,7 +687,7 @@
         <v>0.97</v>
       </c>
       <c r="E7" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="8">
@@ -695,16 +695,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B8" t="str">
-        <v>600580</v>
+        <v>601598</v>
       </c>
       <c r="C8" t="str">
-        <v>卧龙电驱</v>
+        <v>中国外运</v>
       </c>
       <c r="D8">
-        <v>5.89</v>
+        <v>10</v>
       </c>
       <c r="E8" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="9">
@@ -712,16 +712,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B9" t="str">
-        <v>601598</v>
+        <v>601878</v>
       </c>
       <c r="C9" t="str">
-        <v>中国外运</v>
+        <v>浙商证券</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>4.84</v>
       </c>
       <c r="E9" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="10">
@@ -729,16 +729,16 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B10" t="str">
-        <v>601878</v>
+        <v>603119</v>
       </c>
       <c r="C10" t="str">
-        <v>浙商证券</v>
+        <v>浙江荣泰</v>
       </c>
       <c r="D10">
-        <v>4.85</v>
+        <v>0.03</v>
       </c>
       <c r="E10" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="11">
@@ -746,38 +746,21 @@
         <v>大成 (锐进先锋)</v>
       </c>
       <c r="B11" t="str">
-        <v>603119</v>
+        <v>HK01810</v>
       </c>
       <c r="C11" t="str">
-        <v>浙江荣泰</v>
+        <v>小米集团-W</v>
       </c>
       <c r="D11">
-        <v>0.03</v>
+        <v>1.01</v>
       </c>
       <c r="E11" t="str">
-        <v>202509241121</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>大成 (锐进先锋)</v>
-      </c>
-      <c r="B12" t="str">
-        <v>HK01810</v>
-      </c>
-      <c r="C12" t="str">
-        <v>小米集团-W</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -832,7 +815,7 @@
         <v>5.06</v>
       </c>
       <c r="G2" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="3">
@@ -855,7 +838,7 @@
         <v>0.99</v>
       </c>
       <c r="G3" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="4">
@@ -875,10 +858,10 @@
         <v>4.96</v>
       </c>
       <c r="F4">
-        <v>5.08</v>
+        <v>5.1</v>
       </c>
       <c r="G4" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="5">
@@ -901,7 +884,7 @@
         <v>9.28</v>
       </c>
       <c r="G5" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="6">
@@ -924,7 +907,7 @@
         <v>6.94</v>
       </c>
       <c r="G6" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="7">
@@ -947,7 +930,7 @@
         <v>1.01</v>
       </c>
       <c r="G7" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="8">
@@ -967,10 +950,10 @@
         <v>5.28</v>
       </c>
       <c r="F8">
-        <v>5.38</v>
+        <v>5.39</v>
       </c>
       <c r="G8" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="9">
@@ -990,10 +973,10 @@
         <v>5.05</v>
       </c>
       <c r="F9">
-        <v>3.21</v>
+        <v>3.19</v>
       </c>
       <c r="G9" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="10">
@@ -1016,7 +999,7 @@
         <v>0.98</v>
       </c>
       <c r="G10" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="11">
@@ -1039,7 +1022,7 @@
         <v>5.06</v>
       </c>
       <c r="G11" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="12">
@@ -1062,7 +1045,7 @@
         <v>1.02</v>
       </c>
       <c r="G12" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
     <row r="13">
@@ -1085,7 +1068,7 @@
         <v>0.97</v>
       </c>
       <c r="G13" t="str">
-        <v>202509241121</v>
+        <v>202509250137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>